<commit_message>
Add SOA CoreService Name
</commit_message>
<xml_diff>
--- a/ReSTAPI/BNI CBS Rest API.xlsx
+++ b/ReSTAPI/BNI CBS Rest API.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9F949A-6CC1-4544-B96B-B6D1D9D641BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43640BBF-8548-4130-A6B4-3EAFC5412415}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="107">
   <si>
     <t>CreateTapenasDepositAccount</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>055675.xml</t>
-  </si>
-  <si>
-    <t>000400.xml</t>
   </si>
   <si>
     <t>032070.xml</t>
@@ -384,12 +381,124 @@
   <si>
     <t>type of beneficiary = tipeResidensiPenerima</t>
   </si>
+  <si>
+    <t>--invalid core service--</t>
+  </si>
+  <si>
+    <t>CreateTopUpAccount</t>
+  </si>
+  <si>
+    <t>SOA Core Service Name</t>
+  </si>
+  <si>
+    <t>CreateDepositAccount</t>
+  </si>
+  <si>
+    <t>HistoricalTransactions</t>
+  </si>
+  <si>
+    <t>AccountShortInquiry 
+AccountShortDetails</t>
+  </si>
+  <si>
+    <t>DebitCardDetails</t>
+  </si>
+  <si>
+    <t>GetCardByAccount</t>
+  </si>
+  <si>
+    <t>CifDetails
+GetPersonalInfo</t>
+  </si>
+  <si>
+    <t>CustomerDetailV2</t>
+  </si>
+  <si>
+    <t>OpenAccountList</t>
+  </si>
+  <si>
+    <t>KliringOutwardV2</t>
+  </si>
+  <si>
+    <t>DepositTransfer</t>
+  </si>
+  <si>
+    <t>RtgsOutward</t>
+  </si>
+  <si>
+    <t>--no core service 000400--</t>
+  </si>
+  <si>
+    <t>TermDepositRateInquiry</t>
+  </si>
+  <si>
+    <t>--no core service 002071--</t>
+  </si>
+  <si>
+    <t xml:space="preserve">additional premium (dropdown) 
+insurance clain payment (dropdown) 
+</t>
+  </si>
+  <si>
+    <t>Deposit: .xml
+Loan: .xml
+Tappenas: .xml 
+Deposito: .xml 
+Haji: .xml</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">000400.xml
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>069400.xml</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Loan: .xml
+</t>
+  </si>
+  <si>
+    <t>Refer to 069400.xml at no #4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please use 069491.xml and applied to any customer type
+</t>
+  </si>
+  <si>
+    <t>butuh xsd SOA, request &amp; response</t>
+  </si>
+  <si>
+    <t>Type of Beneficiary (dropdown)</t>
+  </si>
+  <si>
+    <t>Additional Premium 
+Term 
+Maturity Date (Due Date)</t>
+  </si>
+  <si>
+    <t>Detail informasi transcode 2071 &amp; responsenya</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,6 +570,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -505,7 +627,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -537,6 +659,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2684,24 +2812,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE31A936-F5C6-4001-9455-E7E19AE8D933}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="83" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.54296875" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="50.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="23.54296875" style="5"/>
+    <col min="2" max="3" width="36.54296875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="50.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="23.54296875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -2709,19 +2837,22 @@
         <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="40.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2729,19 +2860,25 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="G2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2749,19 +2886,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="G3" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2769,19 +2909,22 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2789,19 +2932,25 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="94.5" x14ac:dyDescent="0.35">
+      <c r="F5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2809,19 +2958,25 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2829,19 +2984,22 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="G7" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2849,19 +3007,22 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="54" x14ac:dyDescent="0.35">
+      <c r="G8" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="54" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2869,19 +3030,22 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="G9" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="54" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2889,19 +3053,25 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="F10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2909,22 +3079,28 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.35">
+      <c r="I11" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="27" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2932,39 +3108,48 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.35">
+      <c r="G12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="27" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="F13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G13" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2972,17 +3157,20 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" ht="27" x14ac:dyDescent="0.35">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="27" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2990,39 +3178,54 @@
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="G15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>65</v>
+      <c r="C16" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="G16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3030,33 +3233,42 @@
         <v>16</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="27" x14ac:dyDescent="0.35">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" ht="27" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>67</v>
+      <c r="C18" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="27" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="I18" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="27" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3064,25 +3276,28 @@
         <v>19</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{79FBCB4B-F805-4E26-B2A7-4CDFFE1B9984}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{F460D41D-FA4F-457B-980C-C51038979E60}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{2C971A67-9768-4112-AB94-7CA9C74414DB}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{5BFD549C-CD64-47E2-A95A-26F6176D00EC}"/>
-    <hyperlink ref="F7" r:id="rId5" xr:uid="{C6471BCD-2DF2-49F7-A96D-DD947B5EE5CA}"/>
-    <hyperlink ref="F8" r:id="rId6" xr:uid="{ED230618-2D01-4C28-B1B5-251118E6017E}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{222D47E2-901F-4672-9986-E6EBAE8C5693}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{79FBCB4B-F805-4E26-B2A7-4CDFFE1B9984}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{F460D41D-FA4F-457B-980C-C51038979E60}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{2C971A67-9768-4112-AB94-7CA9C74414DB}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{5BFD549C-CD64-47E2-A95A-26F6176D00EC}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{C6471BCD-2DF2-49F7-A96D-DD947B5EE5CA}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{ED230618-2D01-4C28-B1B5-251118E6017E}"/>
+    <hyperlink ref="G10" r:id="rId7" xr:uid="{222D47E2-901F-4672-9986-E6EBAE8C5693}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -3093,8 +3308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054E4152-3998-4793-B440-5454AADA64C4}">
   <dimension ref="A2:C514"/>
   <sheetViews>
-    <sheetView topLeftCell="A378" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B227" sqref="B227"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3153,7 +3368,7 @@
     </row>
     <row r="69" spans="3:3" ht="21" x14ac:dyDescent="0.5">
       <c r="C69" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -3164,7 +3379,7 @@
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
@@ -3175,12 +3390,12 @@
         <v>3</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="141" spans="3:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C141" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
@@ -3209,17 +3424,17 @@
     </row>
     <row r="189" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C189" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="211" spans="3:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C211" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="232" spans="3:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C232" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">

</xml_diff>